<commit_message>
Cập nhật Activity_Table lần 1
</commit_message>
<xml_diff>
--- a/Activity_Table.xlsx
+++ b/Activity_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -108,13 +108,28 @@
   </si>
   <si>
     <t>Code module chức năng thống kê</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Kiểm thử các module</t>
+  </si>
+  <si>
+    <t>E, F, G, H, I, J, K</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Báo cáo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +165,11 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="3">
@@ -198,7 +218,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -221,6 +241,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="3" builtinId="26"/>
@@ -229,9 +255,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -291,17 +314,20 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thick">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thick">
           <color theme="4" tint="0.499984740745262"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thick">
-          <color theme="4"/>
-        </top>
-      </border>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -317,13 +343,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A2:D13" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" headerRowCellStyle="Heading 2">
-  <autoFilter ref="A2:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A2:D15" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" headerRowCellStyle="Heading 2">
+  <autoFilter ref="A2:D15"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="ID" dataDxfId="4" dataCellStyle="Good"/>
-    <tableColumn id="2" name="Hoạt động" dataDxfId="3"/>
-    <tableColumn id="3" name="Số ngày" dataDxfId="2"/>
-    <tableColumn id="4" name="Hoạt động trước" dataDxfId="1"/>
+    <tableColumn id="1" name="ID" dataDxfId="3" dataCellStyle="Good"/>
+    <tableColumn id="2" name="Hoạt động" dataDxfId="2"/>
+    <tableColumn id="3" name="Số ngày" dataDxfId="1"/>
+    <tableColumn id="4" name="Hoạt động trước" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -592,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,6 +808,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="14" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Cập nhật Activity Table lần 2
</commit_message>
<xml_diff>
--- a/Activity_Table.xlsx
+++ b/Activity_Table.xlsx
@@ -107,9 +107,6 @@
     <t>Code module quản lý hoá đơn</t>
   </si>
   <si>
-    <t>Code module chức năng thống kê</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Báo cáo</t>
+  </si>
+  <si>
+    <t>Code module quản lý tài khoản</t>
   </si>
 </sst>
 </file>
@@ -238,14 +238,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -621,7 +621,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,12 +633,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -798,42 +798,42 @@
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="C14" s="9">
-        <v>1</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>28</v>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chinh sua Activity_Table: Tang thoi gian Code Module
</commit_message>
<xml_diff>
--- a/Activity_Table.xlsx
+++ b/Activity_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\GitHub\HQN-Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E270A2B5-190F-42A0-8A5E-BBB81A6705CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB03CEA1-299F-4FA5-9DFA-382350A5A6FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="3225" windowWidth="13320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="2655" windowWidth="13320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -643,7 +643,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +782,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>15</v>
@@ -796,7 +796,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>15</v>
@@ -810,7 +810,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>15</v>
@@ -824,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>15</v>
@@ -838,7 +838,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>15</v>
@@ -852,7 +852,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>15</v>
@@ -866,7 +866,7 @@
         <v>29</v>
       </c>
       <c r="C16" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>15</v>

</xml_diff>